<commit_message>
Atualização de Capas, Logos e Titulos da plataforma
</commit_message>
<xml_diff>
--- a/Imgs_Jogos/Infomacoes_Jogos.xlsx
+++ b/Imgs_Jogos/Infomacoes_Jogos.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24131"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24228"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Victor Luz\Desktop\Blue\Repositório Módulo 1\GitHub\projeto-gameflix-blue\Imgs_Jogos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2403C31F-4F02-49BC-B04B-A5805BCA5440}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DF50A895-CBF0-442B-A6AC-AF6C5CD0DC49}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="480" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="100">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="118">
   <si>
     <t>Nome</t>
   </si>
@@ -33,9 +33,6 @@
     <t>Nota Metacritc</t>
   </si>
   <si>
-    <t>Classificação</t>
-  </si>
-  <si>
     <t>Genero</t>
   </si>
   <si>
@@ -49,9 +46,6 @@
   </si>
   <si>
     <t>9.5</t>
-  </si>
-  <si>
-    <t>Ação</t>
   </si>
   <si>
     <t>https://www.youtube.com/watch?v=CJ_GCPaKywg</t>
@@ -206,9 +200,6 @@
     <t>https://www.youtube.com/watch?v=DHHcM6aHPnE</t>
   </si>
   <si>
-    <t>Assassin´s Creed – Black Flag</t>
-  </si>
-  <si>
     <t>Assassin’s Creed 4: Black Flag é o mais recente título de uma das franquias de maior sucesso da atualidade. O game da Ubisoft transporta o jogador para um tema nunca antes abordado pela série: piratas. O jogo está disponível tanto para os consoles da nova geração, Xbox One e PS4 quanto para PlayStation 3, Xbox 360, PC e Wii U. Navegue pelos mares caribenhos e se aventure neste repleto mundo aberto na pele do pirata Edward Kenway.</t>
   </si>
   <si>
@@ -336,6 +327,69 @@
   </si>
   <si>
     <t>Mobile Legends : Bang Bang</t>
+  </si>
+  <si>
+    <t>8.8</t>
+  </si>
+  <si>
+    <t>Blizzard Entertainment</t>
+  </si>
+  <si>
+    <t>Diablo II: Resurrected</t>
+  </si>
+  <si>
+    <t>Diablo 2 é um RPG dividido em 4 atos, com seus cenários vastos para sua exploração. O seu objetivo assim como seu antecessor é eliminar as hordas de monstros, juntamente com os outros senhores do inferno, apresentados em cada atos do jogo ligados com cenas cinematográficas impressionantes. Hoje 20 anos depois, surge com sua forma remasterizada para todas as plataformas, além de gráficos em até 4k, além de melhorias em sua jogabilidade.</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=NxgSXPj75m4</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=-wYSsnKRbRY</t>
+  </si>
+  <si>
+    <t>Resident Evil / Biohazard - HD Remaster</t>
+  </si>
+  <si>
+    <t>Descrição:  Uma obra-prima criada por Shinji Mikami. Jogo começa com uma das mains icônicas openings até hoje, onde os membros da S.T.A.R.S – uma equipe de resgate foi enviada para investigar da equipe Alpha desaparecidos pela floresta de Raccoon City. Assumindo o controle dos agentes Chris Redfield ou Jill Valentine descubra os segredos por trás de uma instalação de pesquisa genética radical. Com uma série de armas para dominar e horrores em cada esquina, o teste final pode ser apenas para sair vivo.</t>
+  </si>
+  <si>
+    <t>Survival Horror</t>
+  </si>
+  <si>
+    <t>Capcom</t>
+  </si>
+  <si>
+    <t>Ghost of Tsushima</t>
+  </si>
+  <si>
+    <t>O ano é 1274. Guerreiros samurais são os lendários defensores do Japão, até que o temível Império Mongol invade a ilha de Tsushima, causando estragos e conquistando a população local. Como um dos últimos samurais sobreviventes, você se levanta das cinzas para lutar. Mas táticas honrosas não o levarão à vitória. Você deve ir além de suas tradições samurais para forjar uma nova maneira de lutar, o caminho do Fantasma, enquanto trava uma guerra não convencional pela liberdade do Japão.</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=iqysmS4lxwQ</t>
+  </si>
+  <si>
+    <t>Action Adventure</t>
+  </si>
+  <si>
+    <t>Parasite Eve</t>
+  </si>
+  <si>
+    <t>Um deles é um policial. O outro está possuído por um antigo mal ameaçando toda a vida na Terra. O terrível vínculo entre eles continuará até que algo morra. Uma aventura arrepiante que só poderia vir dos criadores de Final Fantasy VII. Um conto épico de ficção científica contada através de impressionantes sequências renderizadas em 3D. Monstros mutantes de batalha em combate de polígono em tempo real. Personalize armas, armaduras e habilidades de caráter.</t>
+  </si>
+  <si>
+    <t>SquareSoft</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=WLQCY3_DK58</t>
+  </si>
+  <si>
+    <t>8.1</t>
+  </si>
+  <si>
+    <t>Classificação (Anos)</t>
+  </si>
+  <si>
+    <t>Assassin´s Creed IV– Black Flag</t>
   </si>
 </sst>
 </file>
@@ -410,7 +464,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -428,6 +482,12 @@
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -711,10 +771,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H20"/>
+  <dimension ref="A1:H22"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="A13" sqref="A13"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -734,511 +794,601 @@
         <v>0</v>
       </c>
       <c r="B1" s="5" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C1" s="5" t="s">
         <v>1</v>
       </c>
       <c r="D1" s="5" t="s">
+        <v>116</v>
+      </c>
+      <c r="E1" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="5" t="s">
+      <c r="F1" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="5" t="s">
+      <c r="G1" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="5" t="s">
+      <c r="H1" s="5" t="s">
         <v>5</v>
-      </c>
-      <c r="H1" s="5" t="s">
-        <v>6</v>
       </c>
     </row>
     <row r="2" spans="1:8" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="D2" s="1">
         <v>12</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="F2" s="1">
         <v>2020</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="H2" s="6" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
     </row>
     <row r="3" spans="1:8" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
-        <v>58</v>
+        <v>117</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="D3" s="1">
         <v>18</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>8</v>
+        <v>110</v>
       </c>
       <c r="F3" s="1">
         <v>2013</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="H3" s="6" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
     </row>
     <row r="4" spans="1:8" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="B4" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="B4" s="1" t="s">
-        <v>91</v>
-      </c>
       <c r="C4" s="1" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="D4" s="1">
         <v>12</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="F4" s="1">
         <v>2013</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="H4" s="6" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
     </row>
     <row r="5" spans="1:8" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="C5" s="1" t="s">
         <v>37</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>39</v>
       </c>
       <c r="D5" s="1">
         <v>18</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="F5" s="1">
         <v>2016</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="H5" s="6" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
     </row>
     <row r="6" spans="1:8" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="C6" s="1" t="s">
         <v>42</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>44</v>
       </c>
       <c r="D6" s="1">
         <v>16</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="F6" s="1">
         <v>2020</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="H6" s="6" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="7" spans="1:8" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="D7" s="1">
         <v>18</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="F7" s="1">
         <v>2008</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="H7" s="6" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
     </row>
     <row r="8" spans="1:8" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="4" t="s">
+      <c r="A8" s="3" t="s">
+        <v>99</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="D8" s="1">
+        <v>17</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="F8" s="1">
+        <v>2000</v>
+      </c>
+      <c r="G8" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="H8" s="6" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="D9" s="1">
+        <v>12</v>
+      </c>
+      <c r="E9" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="F9" s="1">
+        <v>2016</v>
+      </c>
+      <c r="G9" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="H9" s="6" t="s">
         <v>74</v>
       </c>
-      <c r="B8" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="C8" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="D8" s="1">
-        <v>12</v>
-      </c>
-      <c r="E8" s="2" t="s">
-        <v>55</v>
-      </c>
-      <c r="F8" s="1">
-        <v>2016</v>
-      </c>
-      <c r="G8" s="1" t="s">
-        <v>76</v>
-      </c>
-      <c r="H8" s="6" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="B9" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="C9" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="D9" s="1">
-        <v>18</v>
-      </c>
-      <c r="E9" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="F9" s="1">
-        <v>2018</v>
-      </c>
-      <c r="G9" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="H9" s="6" t="s">
-        <v>9</v>
-      </c>
     </row>
     <row r="10" spans="1:8" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="B10" s="1" t="s">
-        <v>29</v>
+      <c r="A10" s="8" t="s">
+        <v>107</v>
+      </c>
+      <c r="B10" s="7" t="s">
+        <v>108</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>15</v>
+        <v>57</v>
       </c>
       <c r="D10" s="1">
         <v>18</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>90</v>
+        <v>110</v>
       </c>
       <c r="F10" s="1">
-        <v>2008</v>
+        <v>2020</v>
       </c>
       <c r="G10" s="1" t="s">
-        <v>16</v>
+        <v>31</v>
       </c>
       <c r="H10" s="6" t="s">
-        <v>17</v>
+        <v>109</v>
       </c>
     </row>
     <row r="11" spans="1:8" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
-        <v>63</v>
+        <v>22</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>64</v>
+        <v>25</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>44</v>
+        <v>6</v>
       </c>
       <c r="D11" s="1">
-        <v>12</v>
+        <v>18</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>65</v>
+        <v>18</v>
       </c>
       <c r="F11" s="1">
-        <v>2008</v>
+        <v>2018</v>
       </c>
       <c r="G11" s="1" t="s">
-        <v>66</v>
+        <v>31</v>
       </c>
       <c r="H11" s="6" t="s">
-        <v>67</v>
+        <v>7</v>
       </c>
     </row>
     <row r="12" spans="1:8" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
-        <v>47</v>
+        <v>12</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>48</v>
+        <v>27</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>49</v>
+        <v>13</v>
       </c>
       <c r="D12" s="1">
+        <v>18</v>
+      </c>
+      <c r="E12" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="F12" s="1">
+        <v>2008</v>
+      </c>
+      <c r="G12" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="E12" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="F12" s="1">
-        <v>2004</v>
-      </c>
-      <c r="G12" s="1" t="s">
-        <v>51</v>
-      </c>
       <c r="H12" s="6" t="s">
-        <v>52</v>
+        <v>15</v>
       </c>
     </row>
     <row r="13" spans="1:8" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
-        <v>99</v>
+        <v>60</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>79</v>
+        <v>61</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>81</v>
+        <v>42</v>
       </c>
       <c r="D13" s="1">
         <v>12</v>
       </c>
       <c r="E13" s="2" t="s">
-        <v>80</v>
+        <v>62</v>
       </c>
       <c r="F13" s="1">
-        <v>2016</v>
+        <v>2008</v>
       </c>
       <c r="G13" s="1" t="s">
-        <v>82</v>
+        <v>63</v>
       </c>
       <c r="H13" s="6" t="s">
-        <v>78</v>
+        <v>64</v>
       </c>
     </row>
     <row r="14" spans="1:8" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
-        <v>10</v>
+        <v>45</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>26</v>
+        <v>46</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>12</v>
+        <v>47</v>
       </c>
       <c r="D14" s="1">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="E14" s="2" t="s">
-        <v>36</v>
+        <v>48</v>
       </c>
       <c r="F14" s="1">
-        <v>2017</v>
+        <v>2004</v>
       </c>
       <c r="G14" s="1" t="s">
-        <v>11</v>
+        <v>49</v>
       </c>
       <c r="H14" s="6" t="s">
-        <v>13</v>
+        <v>50</v>
       </c>
     </row>
     <row r="15" spans="1:8" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
-        <v>92</v>
+        <v>96</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>97</v>
+        <v>76</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>94</v>
+        <v>78</v>
       </c>
       <c r="D15" s="1">
         <v>12</v>
       </c>
       <c r="E15" s="2" t="s">
-        <v>98</v>
+        <v>77</v>
       </c>
       <c r="F15" s="1">
         <v>2016</v>
       </c>
       <c r="G15" s="1" t="s">
-        <v>93</v>
+        <v>79</v>
       </c>
       <c r="H15" s="6" t="s">
-        <v>95</v>
+        <v>75</v>
       </c>
     </row>
     <row r="16" spans="1:8" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="3" t="s">
-        <v>83</v>
-      </c>
-      <c r="B16" s="1" t="s">
-        <v>86</v>
+      <c r="A16" s="8" t="s">
+        <v>111</v>
+      </c>
+      <c r="B16" s="7" t="s">
+        <v>112</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>85</v>
+        <v>115</v>
       </c>
       <c r="D16" s="1">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="E16" s="2" t="s">
-        <v>90</v>
+        <v>105</v>
       </c>
       <c r="F16" s="1">
-        <v>2011</v>
+        <v>1998</v>
       </c>
       <c r="G16" s="1" t="s">
-        <v>87</v>
+        <v>113</v>
       </c>
       <c r="H16" s="6" t="s">
-        <v>84</v>
+        <v>114</v>
       </c>
     </row>
     <row r="17" spans="1:8" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="3" t="s">
-        <v>28</v>
+        <v>8</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="D17" s="2">
-        <v>18</v>
+        <v>10</v>
+      </c>
+      <c r="D17" s="1">
+        <v>16</v>
       </c>
       <c r="E17" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="F17" s="1">
-        <v>2015</v>
+        <v>2017</v>
       </c>
       <c r="G17" s="1" t="s">
-        <v>32</v>
+        <v>9</v>
       </c>
       <c r="H17" s="6" t="s">
-        <v>34</v>
+        <v>11</v>
       </c>
     </row>
     <row r="18" spans="1:8" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="3" t="s">
-        <v>53</v>
+        <v>89</v>
       </c>
       <c r="B18" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="D18" s="1">
+        <v>12</v>
+      </c>
+      <c r="E18" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="F18" s="1">
+        <v>2016</v>
+      </c>
+      <c r="G18" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="H18" s="6" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="3" t="s">
+        <v>103</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="D19" s="1">
+        <v>18</v>
+      </c>
+      <c r="E19" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="F19" s="1">
+        <v>2002</v>
+      </c>
+      <c r="G19" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="H19" s="6" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="D20" s="1">
+        <v>12</v>
+      </c>
+      <c r="E20" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="F20" s="1">
+        <v>2011</v>
+      </c>
+      <c r="G20" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="H20" s="6" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="D21" s="2">
+        <v>18</v>
+      </c>
+      <c r="E21" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="F21" s="1">
+        <v>2015</v>
+      </c>
+      <c r="G21" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="H21" s="6" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="D22" s="1">
+        <v>14</v>
+      </c>
+      <c r="E22" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="F22" s="1">
+        <v>2011</v>
+      </c>
+      <c r="G22" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="C18" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="D18" s="1">
-        <v>14</v>
-      </c>
-      <c r="E18" s="2" t="s">
+      <c r="H22" s="6" t="s">
         <v>55</v>
       </c>
-      <c r="F18" s="1">
-        <v>2011</v>
-      </c>
-      <c r="G18" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="H18" s="6" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A19" s="1"/>
-      <c r="B19" s="1"/>
-      <c r="C19" s="1"/>
-      <c r="D19" s="1"/>
-      <c r="E19" s="1"/>
-      <c r="F19" s="1"/>
-      <c r="G19" s="1"/>
-    </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A20" s="1"/>
-      <c r="B20" s="1"/>
-      <c r="C20" s="1"/>
-      <c r="D20" s="1"/>
-      <c r="E20" s="1"/>
-      <c r="F20" s="1"/>
-      <c r="G20" s="1"/>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:H18">
-    <sortCondition ref="A2:A18"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:H22">
+    <sortCondition ref="A2:A22"/>
   </sortState>
   <hyperlinks>
-    <hyperlink ref="H17" r:id="rId1" xr:uid="{F35E6558-E9DF-42EB-A5EA-E18F5987E459}"/>
+    <hyperlink ref="H21" r:id="rId1" xr:uid="{F35E6558-E9DF-42EB-A5EA-E18F5987E459}"/>
     <hyperlink ref="H7" r:id="rId2" xr:uid="{300F577A-606C-432E-BC4C-805E96064987}"/>
-    <hyperlink ref="H10" r:id="rId3" xr:uid="{C4D2B144-BC46-4545-A3DD-F0337056BDB7}"/>
-    <hyperlink ref="H14" r:id="rId4" xr:uid="{DD60A14B-EF83-4614-995C-B01726297675}"/>
-    <hyperlink ref="H9" r:id="rId5" xr:uid="{4C4B52E1-9A71-4232-9A54-2B3084C5B5AD}"/>
+    <hyperlink ref="H12" r:id="rId3" xr:uid="{C4D2B144-BC46-4545-A3DD-F0337056BDB7}"/>
+    <hyperlink ref="H17" r:id="rId4" xr:uid="{DD60A14B-EF83-4614-995C-B01726297675}"/>
+    <hyperlink ref="H11" r:id="rId5" xr:uid="{4C4B52E1-9A71-4232-9A54-2B3084C5B5AD}"/>
     <hyperlink ref="H5" r:id="rId6" xr:uid="{5B2F06BF-1BE2-43DE-AA01-714AAEF01658}"/>
     <hyperlink ref="H6" r:id="rId7" xr:uid="{1016F310-E8B8-4589-BA4B-8091B56EC25D}"/>
-    <hyperlink ref="H12" r:id="rId8" xr:uid="{8D65B62B-D3EB-47D7-945D-F2D91A86163A}"/>
-    <hyperlink ref="H18" r:id="rId9" xr:uid="{C89A6313-AD85-49D1-B726-E0C84F69E9C9}"/>
+    <hyperlink ref="H14" r:id="rId8" xr:uid="{8D65B62B-D3EB-47D7-945D-F2D91A86163A}"/>
+    <hyperlink ref="H22" r:id="rId9" xr:uid="{C89A6313-AD85-49D1-B726-E0C84F69E9C9}"/>
     <hyperlink ref="H3" r:id="rId10" xr:uid="{8905FEB3-51C4-49EB-BD59-858AEE97E3DA}"/>
-    <hyperlink ref="H11" r:id="rId11" xr:uid="{88682465-DB4D-41B4-8EB9-4356A2DF64A6}"/>
+    <hyperlink ref="H13" r:id="rId11" xr:uid="{88682465-DB4D-41B4-8EB9-4356A2DF64A6}"/>
     <hyperlink ref="H2" r:id="rId12" xr:uid="{A434EE62-6E0C-4D63-BA2E-97935A6752A2}"/>
-    <hyperlink ref="H8" r:id="rId13" xr:uid="{46B3D922-F956-492F-A141-6B3C51DDFA22}"/>
-    <hyperlink ref="H13" r:id="rId14" xr:uid="{F5967909-8054-4D88-9237-2B320F9F8B8E}"/>
-    <hyperlink ref="H16" r:id="rId15" xr:uid="{570C8821-75E4-419D-B6AA-6FDE4D4B5396}"/>
+    <hyperlink ref="H9" r:id="rId13" xr:uid="{46B3D922-F956-492F-A141-6B3C51DDFA22}"/>
+    <hyperlink ref="H15" r:id="rId14" xr:uid="{F5967909-8054-4D88-9237-2B320F9F8B8E}"/>
+    <hyperlink ref="H20" r:id="rId15" xr:uid="{570C8821-75E4-419D-B6AA-6FDE4D4B5396}"/>
     <hyperlink ref="H4" r:id="rId16" xr:uid="{266425EE-6B38-43CE-AD64-6761F1300C12}"/>
-    <hyperlink ref="H15" r:id="rId17" xr:uid="{DE0FF6B7-448A-430F-91ED-8AAFD0755B56}"/>
+    <hyperlink ref="H18" r:id="rId17" xr:uid="{DE0FF6B7-448A-430F-91ED-8AAFD0755B56}"/>
+    <hyperlink ref="H8" r:id="rId18" xr:uid="{C5AD9B38-D0B9-45E5-A8AF-BDEBF23EF1C7}"/>
+    <hyperlink ref="H19" r:id="rId19" xr:uid="{5B44584A-DCC2-4982-AF42-293970BC623A}"/>
+    <hyperlink ref="H10" r:id="rId20" xr:uid="{8A3114F9-D578-4EAA-ABEB-424D3EC76415}"/>
+    <hyperlink ref="H16" r:id="rId21" xr:uid="{7C2C4F47-4769-4C09-9CFB-3E97637532D4}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" verticalDpi="300" r:id="rId18"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="300" r:id="rId22"/>
 </worksheet>
 </file>
</xml_diff>